<commit_message>
Bringing remote up to date with my old laptop - last commit from this beast?
</commit_message>
<xml_diff>
--- a/mao.xlsx
+++ b/mao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="286" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="285" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="mao" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Evan Miller</t>
+  </si>
+  <si>
+    <t>Calculus</t>
   </si>
 </sst>
 </file>
@@ -114,10 +117,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A2:B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -129,7 +132,18 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="n">
         <v>1234</v>
       </c>
     </row>

</xml_diff>